<commit_message>
add vscode worksheet for gidapp
</commit_message>
<xml_diff>
--- a/swertres/my_bets.xlsx
+++ b/swertres/my_bets.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="19200" windowHeight="11775"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="19200" windowHeight="11780"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="5" uniqueCount="5">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="6" uniqueCount="6">
   <si>
     <t>DATE - TIME</t>
   </si>
@@ -39,6 +39,9 @@
   </si>
   <si>
     <t>04 tue jun 2019 0</t>
+  </si>
+  <si>
+    <t>09 sun jun 2019 2</t>
   </si>
 </sst>
 </file>
@@ -391,20 +394,20 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:C10"/>
+  <dimension ref="A1:C13"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C11" sqref="C11"/>
+      <selection activeCell="C13" sqref="C13"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="33.5703125" customWidth="1"/>
-    <col min="2" max="2" width="26.140625" customWidth="1"/>
+    <col min="1" max="1" width="33.54296875" customWidth="1"/>
+    <col min="2" max="2" width="26.1796875" customWidth="1"/>
     <col min="3" max="3" width="15" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -415,7 +418,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A2" t="s">
         <v>3</v>
       </c>
@@ -426,7 +429,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:3" x14ac:dyDescent="0.35">
       <c r="B3">
         <v>263</v>
       </c>
@@ -434,7 +437,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:3" x14ac:dyDescent="0.35">
       <c r="B4">
         <v>743</v>
       </c>
@@ -442,7 +445,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:3" x14ac:dyDescent="0.35">
       <c r="B5">
         <v>143</v>
       </c>
@@ -450,7 +453,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="7" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A7" t="s">
         <v>4</v>
       </c>
@@ -461,7 +464,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="8" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:3" x14ac:dyDescent="0.35">
       <c r="B8">
         <v>244</v>
       </c>
@@ -469,7 +472,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="9" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:3" x14ac:dyDescent="0.35">
       <c r="B9">
         <v>246</v>
       </c>
@@ -477,12 +480,31 @@
         <v>5</v>
       </c>
     </row>
-    <row r="10" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:3" x14ac:dyDescent="0.35">
       <c r="B10">
         <v>224</v>
       </c>
       <c r="C10">
         <v>5</v>
+      </c>
+    </row>
+    <row r="12" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A12" t="s">
+        <v>5</v>
+      </c>
+      <c r="B12">
+        <v>713</v>
+      </c>
+      <c r="C12">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="13" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="B13">
+        <v>313</v>
+      </c>
+      <c r="C13">
+        <v>10</v>
       </c>
     </row>
   </sheetData>

</xml_diff>